<commit_message>
implement catelog service (not works yet)
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/Thuan/Work/Project/ecommerce/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A48A3646-0A54-3D4B-B9C3-D32643EE52AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752BE5C8-AC53-C54B-BF49-499EF06B253E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3160" yWindow="2260" windowWidth="28240" windowHeight="17240" xr2:uid="{53693A3D-D864-1445-9FA1-E2BF536B50AA}"/>
   </bookViews>
@@ -33,6 +33,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Each service is a separate app.</t>
+  </si>
+  <si>
+    <t>the auth-service usesthe synchronize mechanism (http) to communicate with the user-service</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,14 +462,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF90EFE-C426-F14B-AB99-F193F4BD9F8E}">
-  <dimension ref="A1"/>
+  <dimension ref="I11:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="118" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="11" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add prometheus und grafana
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/Thuan/Work/Project/ecommerce/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752BE5C8-AC53-C54B-BF49-499EF06B253E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2205FB2-4D41-1544-8AD0-006F5F1E9231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3160" yWindow="2260" windowWidth="28240" windowHeight="17240" xr2:uid="{53693A3D-D864-1445-9FA1-E2BF536B50AA}"/>
   </bookViews>
@@ -134,6 +134,50 @@
         <a:xfrm>
           <a:off x="762000" y="1790700"/>
           <a:ext cx="5080000" cy="3429000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>118389</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>364856</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>92559</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06CF4D53-6812-4535-8BB4-E66E3B678CE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="635000" y="5844152"/>
+          <a:ext cx="3873500" cy="4064000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -464,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF90EFE-C426-F14B-AB99-F193F4BD9F8E}">
   <dimension ref="I11:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="118" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="118" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>